<commit_message>
added logos to pcbs
</commit_message>
<xml_diff>
--- a/BOM/ConductivityBOM.xlsx
+++ b/BOM/ConductivityBOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="94">
   <si>
     <t>Comment</t>
   </si>
@@ -99,9 +99,6 @@
     <t>D1, D2, D3, D4</t>
   </si>
   <si>
-    <t>FAIR-SOD-523F-2_V</t>
-  </si>
-  <si>
     <t>CMP-0881-00001-1</t>
   </si>
   <si>
@@ -301,6 +298,12 @@
   </si>
   <si>
     <t>0011090P1</t>
+  </si>
+  <si>
+    <t>DO-214AC</t>
+  </si>
+  <si>
+    <t>SeeedStudio part has too large footprint.</t>
   </si>
 </sst>
 </file>
@@ -407,9 +410,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -451,7 +462,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -464,6 +475,10 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -476,6 +491,10 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -747,7 +766,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -758,7 +777,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -771,7 +790,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="24" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -797,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -872,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="10">
         <v>302010095</v>
@@ -956,7 +975,7 @@
         <v>302010103</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -966,11 +985,11 @@
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F9" s="3">
         <v>4</v>
@@ -982,24 +1001,24 @@
         <v>304010013</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
@@ -1013,19 +1032,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -1034,24 +1053,24 @@
         <v>7</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -1060,108 +1079,111 @@
         <v>7</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15">
       <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="10">
-        <v>301040046</v>
+      <c r="H13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="3">
         <v>4</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="H15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="H16" s="10">
         <v>301010132</v>
@@ -1169,25 +1191,25 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" s="3">
         <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" s="10">
         <v>301010534</v>
@@ -1195,25 +1217,25 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="H18" s="10">
         <v>301010198</v>
@@ -1221,25 +1243,25 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="H19" s="10">
         <v>301010692</v>
@@ -1247,25 +1269,25 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="H20" s="10">
         <v>301010165</v>
@@ -1273,25 +1295,25 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" s="3">
         <v>3</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="10">
         <v>301010196</v>
@@ -1299,51 +1321,51 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="H23" s="10">
         <v>301010222</v>
@@ -1351,25 +1373,25 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="H24" s="10">
         <v>301010101</v>
@@ -1377,19 +1399,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F25" s="3">
         <v>2</v>
@@ -1398,24 +1420,24 @@
         <v>7</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
@@ -1424,24 +1446,24 @@
         <v>7</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
@@ -1450,12 +1472,12 @@
         <v>7</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15">
       <c r="A30" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>